<commit_message>
GPLIM-4520: Fixes for code review. Fixed issue with pooled tube upload test failing.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwilson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\mercury\mercury\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tube barcode</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Test Library Name Test Tube</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Fragment Size</t>
+  </si>
+  <si>
+    <t>Read Length</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +533,7 @@
     <col min="12" max="12" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -570,8 +579,17 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -614,8 +632,14 @@
       <c r="O2" t="s">
         <v>25</v>
       </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I3" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-4434: Fixed issue with test failing because of an outdated test spreadsheet.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwilson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\mercury\mercury\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tube barcode</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Test Library Name Test Tube</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Fragment Size</t>
+  </si>
+  <si>
+    <t>Read Length</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +533,7 @@
     <col min="12" max="12" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -570,8 +579,17 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -614,8 +632,14 @@
       <c r="O2" t="s">
         <v>25</v>
       </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I3" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-5135 fixes and improvements for Pooled Tube Upload
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\mercury\mercury\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="9520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -173,16 +171,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +324,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,27 +511,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
     <col min="7" max="7" width="51" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -589,7 +587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -632,6 +630,9 @@
       <c r="O2" t="s">
         <v>25</v>
       </c>
+      <c r="P2">
+        <v>61</v>
+      </c>
       <c r="Q2">
         <v>2</v>
       </c>
@@ -639,11 +640,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="20.25" customHeight="1">
       <c r="I3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GPLIM-5135 code review fixes
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="9520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26200" windowHeight="6560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Tube barcode</t>
   </si>
@@ -81,9 +81,6 @@
     <t>canine_jrd_amy_hyp_nimblegen</t>
   </si>
   <si>
-    <t>SM-4B6KX_ROOT</t>
-  </si>
-  <si>
     <t>COLB-123</t>
   </si>
   <si>
@@ -99,18 +96,6 @@
     <t>Canine</t>
   </si>
   <si>
-    <t>Lsd</t>
-  </si>
-  <si>
-    <t>SM-748OO</t>
-  </si>
-  <si>
-    <t>test-888232</t>
-  </si>
-  <si>
-    <t>Test Library Name Test Tube</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
@@ -118,13 +103,40 @@
   </si>
   <si>
     <t>Read Length</t>
+  </si>
+  <si>
+    <t>COLB-124</t>
+  </si>
+  <si>
+    <t>COLAB-P-235</t>
+  </si>
+  <si>
+    <t>BP-ID-568</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>lsid:1</t>
+  </si>
+  <si>
+    <t>lsid:2</t>
+  </si>
+  <si>
+    <t>Feline</t>
+  </si>
+  <si>
+    <t>(unique value filled in by the test)</t>
+  </si>
+  <si>
+    <t>(same as broad sample)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +155,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,11 +213,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -197,11 +233,16 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -501,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,23 +553,27 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1"/>
-    <col min="7" max="7" width="51" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" customWidth="1"/>
-    <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1">
@@ -578,27 +623,27 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -613,22 +658,22 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="P2">
         <v>61</v>
@@ -640,8 +685,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="20.25" customHeight="1">
-      <c r="I3" s="5"/>
+    <row r="3" spans="1:18">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3">
+        <v>62</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GPLIM-5942 remove Pooled Dev Tube experiment and condition
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubeReg.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Tube barcode</t>
   </si>
@@ -45,12 +45,6 @@
     <t>CAT</t>
   </si>
   <si>
-    <t>Experiment</t>
-  </si>
-  <si>
-    <t>Conditions</t>
-  </si>
-  <si>
     <t>Collaborator sample ID</t>
   </si>
   <si>
@@ -67,12 +61,6 @@
   </si>
   <si>
     <t>Lsid</t>
-  </si>
-  <si>
-    <t>DEV-6796</t>
-  </si>
-  <si>
-    <t>DEV-6815, DEV-6816</t>
   </si>
   <si>
     <t>Illumina_P5-Nijow_P7-Waren</t>
@@ -560,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,20 +568,18 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -624,7 +610,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -634,42 +620,36 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -678,94 +658,82 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
       <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2">
+        <v>61</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2">
-        <v>61</v>
-      </c>
-      <c r="Q2">
-        <v>2</v>
-      </c>
-      <c r="R2">
-        <v>4</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3">
+        <v>62</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3">
-        <v>62</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3">
-        <v>4</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="S4" s="6"/>
+    <row r="4" spans="1:17">
+      <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:19">
-      <c r="S5" s="6"/>
+    <row r="5" spans="1:17">
+      <c r="Q5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>